<commit_message>
change data to one only
</commit_message>
<xml_diff>
--- a/data/act_veg_by_country.xlsx
+++ b/data/act_veg_by_country.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\CGLS\CGLS_dashboard\mock_up\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work\CGLS\CLMS_website\webtools\webtools\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,18 +22,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="5">
   <si>
     <t>Category</t>
   </si>
   <si>
     <t>AWU: Non-family labour force working on non-regular basis</t>
-  </si>
-  <si>
-    <t>AWU: Family labour force</t>
-  </si>
-  <si>
-    <t>AWU: Regular non family labour force</t>
   </si>
   <si>
     <t>Belgium</t>
@@ -410,73 +404,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="B1:D1048576"/>
+      <selection activeCell="C1" sqref="C1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="102" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="102" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="B2" s="4">
         <v>2880.55</v>
       </c>
-      <c r="C2" s="4">
-        <v>55920.55</v>
-      </c>
-      <c r="D2" s="4">
-        <v>10790.55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="4">
         <v>90.55</v>
       </c>
-      <c r="C3" s="4">
-        <v>3330.55</v>
-      </c>
-      <c r="D3" s="4">
-        <v>560.54999999999995</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="4">
         <v>13360.55</v>
-      </c>
-      <c r="C4" s="4">
-        <v>109690.55</v>
-      </c>
-      <c r="D4" s="4">
-        <v>50880.55</v>
       </c>
     </row>
   </sheetData>
@@ -487,74 +455,48 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:D1048576"/>
+      <selection activeCell="C1" sqref="C1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="5"/>
     <col min="2" max="2" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="102" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="102" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>4</v>
       </c>
       <c r="B2" s="4">
         <v>2970.55</v>
       </c>
-      <c r="C2" s="4">
-        <v>52130.55</v>
-      </c>
-      <c r="D2" s="4">
-        <v>10500.55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="4">
         <v>70.55</v>
       </c>
-      <c r="C3" s="4">
-        <v>3180.55</v>
-      </c>
-      <c r="D3" s="4">
-        <v>500.55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="4">
         <v>14120.55</v>
-      </c>
-      <c r="C4" s="4">
-        <v>100430.55</v>
-      </c>
-      <c r="D4" s="4">
-        <v>50570.55</v>
       </c>
     </row>
   </sheetData>
@@ -564,72 +506,48 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:D1048576"/>
+      <selection activeCell="C1" sqref="C1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="9.140625" style="5"/>
-    <col min="5" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="2" width="9.140625" style="5"/>
+    <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>4</v>
       </c>
       <c r="B2" s="4">
         <v>4120.55</v>
       </c>
-      <c r="C2" s="4">
-        <v>46170.55</v>
-      </c>
-      <c r="D2" s="4">
-        <v>11260.55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="4">
         <v>150.55000000000001</v>
       </c>
-      <c r="C3" s="4">
-        <v>2790.55</v>
-      </c>
-      <c r="D3" s="4">
-        <v>750.55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="4">
         <v>20280.55</v>
-      </c>
-      <c r="C4" s="4">
-        <v>95550.55</v>
-      </c>
-      <c r="D4" s="4">
-        <v>45860.55</v>
       </c>
     </row>
   </sheetData>
@@ -639,72 +557,48 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="9.140625" style="5"/>
-    <col min="5" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="2" width="9.140625" style="5"/>
+    <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>4</v>
       </c>
       <c r="B2" s="4">
         <v>4720.55</v>
       </c>
-      <c r="C2" s="4">
-        <v>40220.550000000003</v>
-      </c>
-      <c r="D2" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="4">
         <v>160.55000000000001</v>
       </c>
-      <c r="C3" s="4">
-        <v>2410.5500000000002</v>
-      </c>
-      <c r="D3" s="4">
-        <v>970.55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="4">
         <v>21550.55</v>
-      </c>
-      <c r="C4" s="4">
-        <v>88730.55</v>
-      </c>
-      <c r="D4" s="4">
-        <v>43020.55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
define excel file template for the countries
</commit_message>
<xml_diff>
--- a/data/act_veg_by_country.xlsx
+++ b/data/act_veg_by_country.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="28620" windowHeight="13170" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="28620" windowHeight="13170" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="2005" sheetId="1" r:id="rId1"/>
+    <sheet name="East Africa" sheetId="1" r:id="rId1"/>
     <sheet name="2007" sheetId="2" r:id="rId2"/>
-    <sheet name="2010" sheetId="3" r:id="rId3"/>
+    <sheet name="Northern Europe" sheetId="3" r:id="rId3"/>
     <sheet name="2013" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621" iterateDelta="1E-4"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="9">
   <si>
     <t>Category</t>
   </si>
@@ -37,6 +37,18 @@
   </si>
   <si>
     <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Performance</t>
+  </si>
+  <si>
+    <t>Ethiopia</t>
+  </si>
+  <si>
+    <t>Eritrea</t>
+  </si>
+  <si>
+    <t>Sweden</t>
   </si>
 </sst>
 </file>
@@ -404,28 +416,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1048576"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="102" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4">
         <v>2880.55</v>
@@ -445,6 +457,14 @@
       </c>
       <c r="B4" s="4">
         <v>13360.55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4">
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -506,24 +526,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="5"/>
+    <col min="1" max="1" width="9.140625" style="5"/>
+    <col min="2" max="2" width="22" style="5" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -534,19 +555,27 @@
         <v>4120.55</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B3" s="4">
-        <v>150.55000000000001</v>
+        <v>370</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>150.55000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B5" s="4">
         <v>20280.55</v>
       </c>
     </row>
@@ -559,7 +588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
test negative values for country performance
</commit_message>
<xml_diff>
--- a/data/act_veg_by_country.xlsx
+++ b/data/act_veg_by_country.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="28620" windowHeight="13170" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="28620" windowHeight="13170" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="East Africa" sheetId="1" r:id="rId1"/>
@@ -478,7 +478,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1048576"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,7 +500,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4">
-        <v>2970.55</v>
+        <v>-2970.55</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">
@@ -528,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,7 +552,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4">
-        <v>4120.55</v>
+        <v>-4120.55</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -588,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,7 +619,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="4">
-        <v>160.55000000000001</v>
+        <v>-160.55000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="25.5" x14ac:dyDescent="0.25">

</xml_diff>